<commit_message>
Added .STL/.STEP files for all hands
</commit_message>
<xml_diff>
--- a/BOM/Macao/Macao_BOM_Control_and_Price_Tracking.xlsx
+++ b/BOM/Macao/Macao_BOM_Control_and_Price_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudy\OneDrive\PhD\VS Code\Prosthetic-Hands\Prosthetic-Hands\BOM\Macao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEF30BE-C8C2-4760-96CF-7C1D5011F94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE95C90-51DD-4A31-87EF-827ED118B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{043B56EA-62B9-4C47-8B29-ED9E1364A12F}"/>
   </bookViews>
@@ -230,10 +230,10 @@
     <t>RS Online</t>
   </si>
   <si>
-    <t>~40 per hand</t>
-  </si>
-  <si>
     <t>BOM Control and Price Tracking - Macao</t>
+  </si>
+  <si>
+    <t>~20 per hand</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1183,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1390,14 +1390,14 @@
         <v>27</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" s="9">
-        <v>0.33</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
-        <v>1.8579000000000001</v>
+        <v>0.94020999999999999</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -1955,7 +1955,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="12">
         <f>SUM($F$4:$F30)</f>
-        <v>334.91090000000003</v>
+        <v>333.99321000000003</v>
       </c>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>

</xml_diff>